<commit_message>
Début passage commande ET début plan de tests
+ Précision plan actuel
</commit_message>
<xml_diff>
--- a/Doc/newPlanning.xlsx
+++ b/Doc/newPlanning.xlsx
@@ -16,21 +16,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Activité/Jour</t>
   </si>
   <si>
-    <t>Conception BDD + Remplissange</t>
-  </si>
-  <si>
-    <t>PHP Programmation</t>
-  </si>
-  <si>
     <t>Journal de bord</t>
   </si>
   <si>
     <t>Documentation</t>
+  </si>
+  <si>
+    <t>Conception BDD + Remplissage</t>
+  </si>
+  <si>
+    <t>index.php</t>
+  </si>
+  <si>
+    <t>Gestock.php</t>
+  </si>
+  <si>
+    <t>DataToHtml.php</t>
+  </si>
+  <si>
+    <t>category.php</t>
+  </si>
+  <si>
+    <t>productDetails.php</t>
+  </si>
+  <si>
+    <t>login.php + Pages liées</t>
+  </si>
+  <si>
+    <t>Scripts ajouter au panier</t>
+  </si>
+  <si>
+    <t>Scripts passer commande</t>
   </si>
 </sst>
 </file>
@@ -92,7 +113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -103,6 +124,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK11"/>
+  <dimension ref="A1:AO16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AI3" sqref="AI3"/>
+      <selection activeCell="Z14" sqref="Z14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,7 +440,7 @@
     <col min="25" max="88" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -470,82 +492,158 @@
       <c r="AE1" s="7"/>
       <c r="AF1" s="7"/>
       <c r="AG1" s="7"/>
-      <c r="AH1" s="1"/>
-      <c r="AI1" s="1"/>
-      <c r="AJ1" s="1"/>
-      <c r="AK1" s="1"/>
-    </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AH1" s="7">
+        <v>9</v>
+      </c>
+      <c r="AI1" s="7"/>
+      <c r="AJ1" s="7"/>
+      <c r="AK1" s="7"/>
+      <c r="AL1" s="7">
+        <v>10</v>
+      </c>
+      <c r="AM1" s="7"/>
+      <c r="AN1" s="7"/>
+      <c r="AO1" s="7"/>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-    </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="T7" s="3"/>
+      <c r="U7" s="8"/>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="6"/>
-      <c r="V10" s="6"/>
-      <c r="W10" s="6"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="5"/>
-      <c r="Z10" s="5"/>
-      <c r="AA10" s="5"/>
-      <c r="AB10" s="5"/>
-      <c r="AC10" s="5"/>
-      <c r="AD10" s="5"/>
-      <c r="AE10" s="5"/>
-      <c r="AF10" s="5"/>
-      <c r="AG10" s="5"/>
-    </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="5"/>
+      <c r="AC14" s="5"/>
+      <c r="AD14" s="5"/>
+      <c r="AE14" s="5"/>
+      <c r="AF14" s="5"/>
+      <c r="AG14" s="5"/>
+      <c r="AH14" s="5"/>
+      <c r="AI14" s="5"/>
+      <c r="AJ14" s="5"/>
+      <c r="AK14" s="5"/>
+      <c r="AL14" s="5"/>
+      <c r="AM14" s="5"/>
+      <c r="AN14" s="5"/>
+      <c r="AO14" s="5"/>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="U15"/>
+      <c r="V15"/>
+      <c r="W15"/>
+      <c r="X15"/>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="U16"/>
+      <c r="V16"/>
+      <c r="W16"/>
+      <c r="X16"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
     <mergeCell ref="Z1:AC1"/>
     <mergeCell ref="AD1:AG1"/>
     <mergeCell ref="B1:E1"/>

</xml_diff>

<commit_message>
Gestion produits + début gestion users.
</commit_message>
<xml_diff>
--- a/Doc/newPlanning.xlsx
+++ b/Doc/newPlanning.xlsx
@@ -121,10 +121,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,66 +444,66 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7">
+      <c r="B1" s="8">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8">
         <v>2</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7">
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8">
         <v>3</v>
       </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7">
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8">
         <v>4</v>
       </c>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7">
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8">
         <v>5</v>
       </c>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7">
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8">
         <v>6</v>
       </c>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7">
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8">
         <v>7</v>
       </c>
-      <c r="AA1" s="7"/>
-      <c r="AB1" s="7"/>
-      <c r="AC1" s="7"/>
-      <c r="AD1" s="7">
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8">
         <v>8</v>
       </c>
-      <c r="AE1" s="7"/>
-      <c r="AF1" s="7"/>
-      <c r="AG1" s="7"/>
-      <c r="AH1" s="7">
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
+      <c r="AG1" s="8"/>
+      <c r="AH1" s="8">
         <v>9</v>
       </c>
-      <c r="AI1" s="7"/>
-      <c r="AJ1" s="7"/>
-      <c r="AK1" s="7"/>
-      <c r="AL1" s="7">
+      <c r="AI1" s="8"/>
+      <c r="AJ1" s="8"/>
+      <c r="AK1" s="8"/>
+      <c r="AL1" s="8">
         <v>10</v>
       </c>
-      <c r="AM1" s="7"/>
-      <c r="AN1" s="7"/>
-      <c r="AO1" s="7"/>
+      <c r="AM1" s="8"/>
+      <c r="AN1" s="8"/>
+      <c r="AO1" s="8"/>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -545,14 +545,14 @@
         <v>10</v>
       </c>
       <c r="T7" s="3"/>
-      <c r="U7" s="8"/>
+      <c r="U7" s="7"/>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="V8" s="8"/>
-      <c r="W8" s="8"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" t="s">

</xml_diff>